<commit_message>
Add GetLargeMessageStorage to resolver_list.xlsx
</commit_message>
<xml_diff>
--- a/resolver_list.xlsx
+++ b/resolver_list.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="74">
   <si>
     <t>TYPE</t>
   </si>
@@ -227,6 +227,12 @@
   </si>
   <si>
     <t>ExternalApp</t>
+  </si>
+  <si>
+    <t>GetLargeMessageStorage</t>
+  </si>
+  <si>
+    <t>large_message_storage_datasource</t>
   </si>
 </sst>
 </file>
@@ -248,17 +254,24 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -272,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -282,14 +295,17 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -980,7 +996,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -1038,7 +1054,7 @@
       <c r="A38" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C38" s="2" t="s">
@@ -1101,10 +1117,10 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C44" s="5" t="s">
@@ -1112,10 +1128,10 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C45" s="5" t="s">
@@ -1123,7 +1139,7 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B46" s="2" t="s">
@@ -1134,10 +1150,10 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C47" s="5" t="s">
@@ -1233,10 +1249,10 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="5" t="s">
+      <c r="A56" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B56" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C56" s="2" t="s">
@@ -1244,10 +1260,10 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="5" t="s">
+      <c r="A57" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="B57" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C57" s="2" t="s">
@@ -1255,7 +1271,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="5" t="s">
+      <c r="A58" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B58" s="5" t="s">
@@ -1266,10 +1282,10 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="5" t="s">
+      <c r="A59" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B59" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C59" s="2" t="s">
@@ -1483,6 +1499,17 @@
       </c>
       <c r="C78" s="2" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new resolvers in list
</commit_message>
<xml_diff>
--- a/resolver_list.xlsx
+++ b/resolver_list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AWS\Shared Folder\hl7-ninja\hl7-ninja-appsync\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AWS\Shared Folder\hl7-ninja\appsync\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="95">
   <si>
     <t>TYPE</t>
   </si>
@@ -294,6 +294,21 @@
   </si>
   <si>
     <t>PurgeQueue</t>
+  </si>
+  <si>
+    <t>PutFunction</t>
+  </si>
+  <si>
+    <t>DeleteFunction</t>
+  </si>
+  <si>
+    <t>transformerFunction</t>
+  </si>
+  <si>
+    <t>bitmapperFunction</t>
+  </si>
+  <si>
+    <t>function_datasource</t>
   </si>
 </sst>
 </file>
@@ -657,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z94"/>
+  <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1393,12 +1408,12 @@
     </row>
     <row r="56" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C56" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C56" s="4" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1407,7 +1422,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>45</v>
@@ -1418,7 +1433,7 @@
         <v>55</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>45</v>
@@ -1429,7 +1444,7 @@
         <v>55</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>45</v>
@@ -1437,10 +1452,10 @@
     </row>
     <row r="60" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>45</v>
@@ -1451,7 +1466,7 @@
         <v>58</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>45</v>
@@ -1462,7 +1477,7 @@
         <v>58</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>45</v>
@@ -1470,10 +1485,10 @@
     </row>
     <row r="63" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>45</v>
@@ -1481,7 +1496,7 @@
     </row>
     <row r="64" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>46</v>
@@ -1495,7 +1510,7 @@
         <v>60</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>45</v>
@@ -1505,8 +1520,8 @@
       <c r="A66" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B66" s="4" t="s">
-        <v>61</v>
+      <c r="B66" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>45</v>
@@ -1516,8 +1531,8 @@
       <c r="A67" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B67" s="3" t="s">
-        <v>54</v>
+      <c r="B67" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>45</v>
@@ -1528,18 +1543,18 @@
         <v>60</v>
       </c>
       <c r="B68" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B69" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A69" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>45</v>
@@ -1547,21 +1562,21 @@
     </row>
     <row r="70" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A71" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>63</v>
+      <c r="A71" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>45</v>
@@ -1569,7 +1584,7 @@
     </row>
     <row r="72" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>46</v>
@@ -1580,10 +1595,10 @@
     </row>
     <row r="73" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>45</v>
@@ -1591,7 +1606,7 @@
     </row>
     <row r="74" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>46</v>
@@ -1602,10 +1617,10 @@
     </row>
     <row r="75" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>45</v>
@@ -1613,7 +1628,7 @@
     </row>
     <row r="76" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>46</v>
@@ -1624,43 +1639,43 @@
     </row>
     <row r="77" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A78" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B78" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A79" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B79" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C77" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A78" s="4" t="s">
+      <c r="C79" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A80" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B80" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B80" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>45</v>
@@ -1668,7 +1683,7 @@
     </row>
     <row r="81" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>46</v>
@@ -1679,10 +1694,10 @@
     </row>
     <row r="82" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>54</v>
+        <v>68</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>45</v>
@@ -1693,7 +1708,7 @@
         <v>69</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>45</v>
@@ -1704,7 +1719,7 @@
         <v>69</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>45</v>
@@ -1712,10 +1727,10 @@
     </row>
     <row r="85" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>45</v>
@@ -1723,101 +1738,156 @@
     </row>
     <row r="86" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B86" s="3" t="s">
+      <c r="B89" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C86" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A87" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A88" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A89" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="C89" s="3" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A91" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A92" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A93" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B90" s="6" t="s">
+      <c r="B93" s="6" t="s">
         <v>85</v>
-      </c>
-      <c r="C90" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A91" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B91" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C91" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A92" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B92" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C92" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A93" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B93" s="6" t="s">
-        <v>88</v>
       </c>
       <c r="C93" s="6" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A94" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B94" s="3" t="s">
+      <c r="A94" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B94" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A95" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C95" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A96" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B96" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A97" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B97" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C94" s="3" t="s">
+      <c r="C97" s="3" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A98" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B98" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A99" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B99" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C99" s="6" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
almost updated the resolver list
</commit_message>
<xml_diff>
--- a/resolver_list.xlsx
+++ b/resolver_list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="97">
   <si>
     <t>TYPE</t>
   </si>
@@ -176,18 +176,12 @@
     <t>messageType</t>
   </si>
   <si>
-    <t>DicomTcpInboundNode</t>
-  </si>
-  <si>
     <t>sendEdges</t>
   </si>
   <si>
     <t>app</t>
   </si>
   <si>
-    <t>DicomTcpOutboundNode</t>
-  </si>
-  <si>
     <t>receiveEdges</t>
   </si>
   <si>
@@ -200,9 +194,6 @@
     <t>receiveMessageType</t>
   </si>
   <si>
-    <t>Hl7MllpOutboundNode</t>
-  </si>
-  <si>
     <t>KmsKey</t>
   </si>
   <si>
@@ -236,9 +227,6 @@
     <t>XTenantSendingNode</t>
   </si>
   <si>
-    <t>CognitoUser</t>
-  </si>
-  <si>
     <t>ExternalApp</t>
   </si>
   <si>
@@ -284,12 +272,6 @@
     <t>appNotifications</t>
   </si>
   <si>
-    <t>NotifyApp</t>
-  </si>
-  <si>
-    <t>NotifyUI</t>
-  </si>
-  <si>
     <t>uiNotifications</t>
   </si>
   <si>
@@ -309,6 +291,30 @@
   </si>
   <si>
     <t>function_datasource</t>
+  </si>
+  <si>
+    <t>sendMessageType</t>
+  </si>
+  <si>
+    <t>instances</t>
+  </si>
+  <si>
+    <t>TenantInfo</t>
+  </si>
+  <si>
+    <t>tenantInfo</t>
+  </si>
+  <si>
+    <t>GetTenant</t>
+  </si>
+  <si>
+    <t>ListApiUsers</t>
+  </si>
+  <si>
+    <t>api_user_datasource</t>
+  </si>
+  <si>
+    <t>ListSnsSubscriptions</t>
   </si>
 </sst>
 </file>
@@ -672,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z99"/>
+  <dimension ref="A1:Z103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -768,10 +774,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>15</v>
+        <v>94</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>16</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
@@ -779,10 +785,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
@@ -790,21 +796,21 @@
         <v>3</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>72</v>
+      <c r="B11" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>73</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
@@ -812,333 +818,241 @@
         <v>3</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>19</v>
+      <c r="B13" s="5" t="s">
+        <v>68</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>79</v>
+        <v>32</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>78</v>
+        <v>33</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
-      <c r="Q29" s="2"/>
-      <c r="R29" s="2"/>
-      <c r="S29" s="2"/>
-      <c r="T29" s="2"/>
-      <c r="U29" s="2"/>
-      <c r="V29" s="2"/>
-      <c r="W29" s="2"/>
-      <c r="X29" s="2"/>
-      <c r="Y29" s="2"/>
-      <c r="Z29" s="2"/>
-    </row>
-    <row r="30" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="2"/>
-      <c r="P30" s="2"/>
-      <c r="Q30" s="2"/>
-      <c r="R30" s="2"/>
-      <c r="S30" s="2"/>
-      <c r="T30" s="2"/>
-      <c r="U30" s="2"/>
-      <c r="V30" s="2"/>
-      <c r="W30" s="2"/>
-      <c r="X30" s="2"/>
-      <c r="Y30" s="2"/>
-      <c r="Z30" s="2"/>
-    </row>
-    <row r="31" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
-      <c r="Q31" s="2"/>
-      <c r="R31" s="2"/>
-      <c r="S31" s="2"/>
-      <c r="T31" s="2"/>
-      <c r="U31" s="2"/>
-      <c r="V31" s="2"/>
-      <c r="W31" s="2"/>
-      <c r="X31" s="2"/>
-      <c r="Y31" s="2"/>
-      <c r="Z31" s="2"/>
-    </row>
-    <row r="32" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
-      <c r="P32" s="2"/>
-      <c r="Q32" s="2"/>
-      <c r="R32" s="2"/>
-      <c r="S32" s="2"/>
-      <c r="T32" s="2"/>
-      <c r="U32" s="2"/>
-      <c r="V32" s="2"/>
-      <c r="W32" s="2"/>
-      <c r="X32" s="2"/>
-      <c r="Y32" s="2"/>
-      <c r="Z32" s="2"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="33" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -1169,139 +1083,231 @@
         <v>21</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>18</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="2"/>
+      <c r="V34" s="2"/>
+      <c r="W34" s="2"/>
+      <c r="X34" s="2"/>
+      <c r="Y34" s="2"/>
+      <c r="Z34" s="2"/>
     </row>
     <row r="35" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="2"/>
+      <c r="S35" s="2"/>
+      <c r="T35" s="2"/>
+      <c r="U35" s="2"/>
+      <c r="V35" s="2"/>
+      <c r="W35" s="2"/>
+      <c r="X35" s="2"/>
+      <c r="Y35" s="2"/>
+      <c r="Z35" s="2"/>
     </row>
     <row r="36" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>14</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2"/>
+      <c r="S36" s="2"/>
+      <c r="T36" s="2"/>
+      <c r="U36" s="2"/>
+      <c r="V36" s="2"/>
+      <c r="W36" s="2"/>
+      <c r="X36" s="2"/>
+      <c r="Y36" s="2"/>
+      <c r="Z36" s="2"/>
     </row>
     <row r="37" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2"/>
+      <c r="S37" s="2"/>
+      <c r="T37" s="2"/>
+      <c r="U37" s="2"/>
+      <c r="V37" s="2"/>
+      <c r="W37" s="2"/>
+      <c r="X37" s="2"/>
+      <c r="Y37" s="2"/>
+      <c r="Z37" s="2"/>
     </row>
     <row r="38" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="44" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>49</v>
+        <v>84</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
     </row>
     <row r="45" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>46</v>
+        <v>85</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
     </row>
     <row r="46" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>45</v>
@@ -1309,10 +1315,10 @@
     </row>
     <row r="47" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>45</v>
@@ -1320,10 +1326,10 @@
     </row>
     <row r="48" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>45</v>
@@ -1331,10 +1337,10 @@
     </row>
     <row r="49" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>45</v>
@@ -1342,10 +1348,10 @@
     </row>
     <row r="50" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>45</v>
@@ -1353,21 +1359,21 @@
     </row>
     <row r="51" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>45</v>
@@ -1375,10 +1381,10 @@
     </row>
     <row r="53" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>45</v>
@@ -1386,10 +1392,10 @@
     </row>
     <row r="54" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>45</v>
@@ -1397,10 +1403,10 @@
     </row>
     <row r="55" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>45</v>
@@ -1408,10 +1414,10 @@
     </row>
     <row r="56" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>45</v>
@@ -1419,10 +1425,10 @@
     </row>
     <row r="57" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>45</v>
@@ -1430,10 +1436,10 @@
     </row>
     <row r="58" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>45</v>
@@ -1441,10 +1447,10 @@
     </row>
     <row r="59" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>45</v>
@@ -1452,10 +1458,10 @@
     </row>
     <row r="60" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>45</v>
@@ -1463,10 +1469,10 @@
     </row>
     <row r="61" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>45</v>
@@ -1474,10 +1480,10 @@
     </row>
     <row r="62" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>45</v>
@@ -1485,10 +1491,10 @@
     </row>
     <row r="63" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>45</v>
@@ -1496,7 +1502,7 @@
     </row>
     <row r="64" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>46</v>
@@ -1507,10 +1513,10 @@
     </row>
     <row r="65" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>45</v>
@@ -1518,10 +1524,10 @@
     </row>
     <row r="66" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>51</v>
+        <v>57</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>45</v>
@@ -1529,10 +1535,10 @@
     </row>
     <row r="67" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>45</v>
@@ -1540,21 +1546,21 @@
     </row>
     <row r="68" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A69" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>46</v>
+      <c r="A69" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>45</v>
@@ -1562,21 +1568,21 @@
     </row>
     <row r="70" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B71" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A71" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>45</v>
@@ -1584,10 +1590,10 @@
     </row>
     <row r="72" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>45</v>
@@ -1595,10 +1601,10 @@
     </row>
     <row r="73" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>45</v>
@@ -1606,10 +1612,10 @@
     </row>
     <row r="74" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>45</v>
@@ -1617,7 +1623,7 @@
     </row>
     <row r="75" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>46</v>
@@ -1628,10 +1634,10 @@
     </row>
     <row r="76" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>45</v>
@@ -1639,10 +1645,10 @@
     </row>
     <row r="77" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>45</v>
@@ -1650,21 +1656,21 @@
     </row>
     <row r="78" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A79" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>51</v>
+      <c r="A79" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>45</v>
@@ -1672,10 +1678,10 @@
     </row>
     <row r="80" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>45</v>
@@ -1683,7 +1689,7 @@
     </row>
     <row r="81" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>46</v>
@@ -1694,10 +1700,10 @@
     </row>
     <row r="82" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>45</v>
@@ -1705,7 +1711,7 @@
     </row>
     <row r="83" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>46</v>
@@ -1716,10 +1722,10 @@
     </row>
     <row r="84" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>45</v>
@@ -1727,10 +1733,10 @@
     </row>
     <row r="85" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>45</v>
@@ -1738,10 +1744,10 @@
     </row>
     <row r="86" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>45</v>
@@ -1749,10 +1755,10 @@
     </row>
     <row r="87" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>45</v>
@@ -1760,7 +1766,7 @@
     </row>
     <row r="88" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>46</v>
@@ -1769,12 +1775,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="C89" s="3" t="s">
         <v>45</v>
@@ -1782,10 +1788,10 @@
     </row>
     <row r="90" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="C90" s="3" t="s">
         <v>45</v>
@@ -1793,101 +1799,145 @@
     </row>
     <row r="91" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B91" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B91" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C91" s="3" t="s">
-        <v>45</v>
+      <c r="C91" s="6" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A92" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>10</v>
+      <c r="A92" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A93" s="3" t="s">
-        <v>75</v>
+      <c r="A93" s="6" t="s">
+        <v>76</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C93" s="6" t="s">
-        <v>76</v>
+        <v>51</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A94" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A95" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A96" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="C96" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A97" s="6" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A97" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B97" s="3" t="s">
+      <c r="B97" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A98" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B98" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C97" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A98" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B98" s="6" t="s">
-        <v>90</v>
-      </c>
       <c r="C98" s="6" t="s">
-        <v>94</v>
+        <v>45</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A99" s="3" t="s">
-        <v>21</v>
+      <c r="A99" s="6" t="s">
+        <v>76</v>
       </c>
       <c r="B99" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C99" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A100" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C100" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A101" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B101" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C101" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A102" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B102" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C102" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A103" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C99" s="6" t="s">
-        <v>94</v>
+      <c r="B103" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C103" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>